<commit_message>
making the indicator species file
</commit_message>
<xml_diff>
--- a/Lullington/indicators/indicator_form.xlsx
+++ b/Lullington/indicators/indicator_form.xlsx
@@ -442,82 +442,82 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>h_bryophytes_lichens</t>
+          <t>(h)_bryophytes_lichens</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>h_ulex_genista</t>
+          <t>(h)_ulex_genista</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cg_non-graminae</t>
+          <t>(cg)_non-graminae</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>h dwarf shrubs</t>
+          <t>(h) dwarf shrubs</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>h graminoids</t>
+          <t>(h) graminoids</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cg3_pos</t>
+          <t>(cg)3_pos</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cg2_pos</t>
+          <t>(cg)2_pos</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>h forbs</t>
+          <t>(h) forbs</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>h exotic species</t>
+          <t>(h) exotic species</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>h Acrocarpous mosses</t>
+          <t>(h) Acrocarpous mosses</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>h bracken</t>
+          <t>(h) bracken</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>cg3_neg5</t>
+          <t>(cg)3_neg5</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>cg3_neg10</t>
+          <t>(cg)3_neg10</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>cg2_neg10</t>
+          <t>(cg)2_neg10</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>h herbaceous</t>
+          <t>(h) herbaceous</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>cg tree scrub</t>
+          <t>(cg) tree scrub</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
manual edits to indicator speceis
</commit_message>
<xml_diff>
--- a/Lullington/indicators/indicator_form.xlsx
+++ b/Lullington/indicators/indicator_form.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q223"/>
+  <dimension ref="A1:Q147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,7 +542,9 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -552,12 +554,16 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -575,12 +581,16 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -648,12 +658,16 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -673,7 +687,9 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
@@ -694,12 +710,16 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -719,7 +739,9 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -740,7 +762,9 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
@@ -749,7 +773,9 @@
       <c r="H11" t="n">
         <v>1</v>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -765,7 +791,9 @@
           <t>barbula convoluta</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -790,12 +818,16 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -815,7 +847,9 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
       <c r="G14" t="n">
         <v>1</v>
       </c>
@@ -844,7 +878,9 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
@@ -863,7 +899,9 @@
           <t>brachythecium rutabulum</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
@@ -890,7 +928,9 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -913,7 +953,9 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
       <c r="G18" t="n">
         <v>1</v>
       </c>
@@ -982,7 +1024,9 @@
           <t>bryum</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
@@ -1155,12 +1199,16 @@
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -1178,12 +1226,16 @@
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
@@ -1201,12 +1253,16 @@
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
@@ -1224,12 +1280,16 @@
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -1245,7 +1305,9 @@
           <t>ceratodon purpureus</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -1270,7 +1332,9 @@
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
@@ -1279,7 +1343,9 @@
       <c r="H33" t="n">
         <v>1</v>
       </c>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -1299,12 +1365,16 @@
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -1326,12 +1396,16 @@
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -1351,12 +1425,16 @@
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -1378,12 +1456,16 @@
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -1401,12 +1483,16 @@
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -1460,7 +1546,9 @@
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
+      <c r="Q40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1470,12 +1558,16 @@
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -1493,12 +1585,16 @@
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -1516,12 +1612,16 @@
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>1</v>
+      </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -1541,7 +1641,9 @@
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
@@ -1585,7 +1687,9 @@
           <t>dicranum scoparium</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
@@ -1633,12 +1737,16 @@
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>1</v>
+      </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
@@ -1659,7 +1767,9 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
@@ -1681,12 +1791,16 @@
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>1</v>
+      </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
@@ -1704,12 +1818,16 @@
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>1</v>
+      </c>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
@@ -1777,7 +1895,9 @@
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
@@ -1786,7 +1906,9 @@
       <c r="H54" t="n">
         <v>1</v>
       </c>
-      <c r="I54" t="inlineStr"/>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
@@ -1802,7 +1924,9 @@
           <t>fissidens dubius</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr"/>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
@@ -1827,12 +1951,16 @@
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
@@ -1873,12 +2001,16 @@
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
@@ -1896,7 +2028,9 @@
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
@@ -1921,14 +2055,18 @@
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
         <v>1</v>
       </c>
       <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
@@ -1946,7 +2084,9 @@
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
@@ -1955,7 +2095,9 @@
       <c r="H61" t="n">
         <v>1</v>
       </c>
-      <c r="I61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
@@ -1973,12 +2115,16 @@
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
@@ -1996,12 +2142,16 @@
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
@@ -2019,12 +2169,16 @@
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr"/>
@@ -2042,12 +2196,16 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
@@ -2065,12 +2223,16 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
@@ -2090,7 +2252,9 @@
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>1</v>
+      </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
@@ -2111,7 +2275,9 @@
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="n">
@@ -2120,7 +2286,9 @@
       <c r="H68" t="n">
         <v>1</v>
       </c>
-      <c r="I68" t="inlineStr"/>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
@@ -2140,7 +2308,9 @@
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>1</v>
+      </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
@@ -2159,7 +2329,9 @@
           <t>homalothecium lutescens</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr"/>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
@@ -2184,12 +2356,16 @@
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
@@ -2207,12 +2383,16 @@
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
+      <c r="I72" t="n">
+        <v>1</v>
+      </c>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
@@ -2230,12 +2410,16 @@
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
@@ -2251,7 +2435,9 @@
           <t>hypnum</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr"/>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
@@ -2276,7 +2462,9 @@
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
@@ -2299,7 +2487,9 @@
           <t>kindbergia praelonga</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr"/>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
@@ -2326,7 +2516,9 @@
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr"/>
@@ -2347,12 +2539,16 @@
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
@@ -2370,7 +2566,9 @@
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="D79" t="n">
+        <v>1</v>
+      </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="n">
@@ -2379,7 +2577,9 @@
       <c r="H79" t="n">
         <v>1</v>
       </c>
-      <c r="I79" t="inlineStr"/>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
@@ -2397,12 +2597,16 @@
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
@@ -2420,7 +2624,9 @@
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="n">
@@ -2429,7 +2635,9 @@
       <c r="H81" t="n">
         <v>1</v>
       </c>
-      <c r="I81" t="inlineStr"/>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
@@ -2447,12 +2655,16 @@
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr"/>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
@@ -2470,7 +2682,9 @@
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="n">
@@ -2501,7 +2715,9 @@
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr"/>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr"/>
@@ -2522,12 +2738,16 @@
       </c>
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
@@ -2545,12 +2765,16 @@
       </c>
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
-      <c r="I86" t="inlineStr"/>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
@@ -2568,12 +2792,16 @@
       </c>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
-      <c r="I87" t="inlineStr"/>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
@@ -2591,12 +2819,16 @@
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
@@ -2614,12 +2846,16 @@
       </c>
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
-      <c r="I89" t="inlineStr"/>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
@@ -2637,12 +2873,16 @@
       </c>
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
-      <c r="I90" t="inlineStr"/>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
@@ -2662,7 +2902,9 @@
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr"/>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
@@ -2683,7 +2925,9 @@
       </c>
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="n">
@@ -2692,7 +2936,9 @@
       <c r="H92" t="n">
         <v>1</v>
       </c>
-      <c r="I92" t="inlineStr"/>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
@@ -2710,12 +2956,16 @@
       </c>
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr"/>
-      <c r="I93" t="inlineStr"/>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
@@ -2733,7 +2983,9 @@
       </c>
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
@@ -2758,12 +3010,16 @@
       </c>
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
@@ -2783,7 +3039,9 @@
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr"/>
@@ -2802,7 +3060,9 @@
           <t>pohlia nutans</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr"/>
+      <c r="B97" t="n">
+        <v>1</v>
+      </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
@@ -2827,7 +3087,9 @@
       </c>
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="n">
@@ -2836,7 +3098,9 @@
       <c r="H98" t="n">
         <v>1</v>
       </c>
-      <c r="I98" t="inlineStr"/>
+      <c r="I98" t="n">
+        <v>1</v>
+      </c>
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
@@ -2854,12 +3118,16 @@
       </c>
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
+      <c r="I99" t="n">
+        <v>1</v>
+      </c>
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
@@ -2877,7 +3145,9 @@
       </c>
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
@@ -2902,12 +3172,16 @@
       </c>
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
+      <c r="I101" t="n">
+        <v>1</v>
+      </c>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
@@ -2925,12 +3199,16 @@
       </c>
       <c r="B102" t="inlineStr"/>
       <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr"/>
+      <c r="I102" t="n">
+        <v>1</v>
+      </c>
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
@@ -2948,12 +3226,16 @@
       </c>
       <c r="B103" t="inlineStr"/>
       <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
-      <c r="I103" t="inlineStr"/>
+      <c r="I103" t="n">
+        <v>1</v>
+      </c>
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
@@ -2994,7 +3276,9 @@
           <t>pseudoscleropodium purum</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr"/>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
@@ -3044,12 +3328,16 @@
       </c>
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="D107" t="n">
+        <v>1</v>
+      </c>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr"/>
+      <c r="I107" t="n">
+        <v>1</v>
+      </c>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
@@ -3067,12 +3355,16 @@
       </c>
       <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="inlineStr"/>
-      <c r="I108" t="inlineStr"/>
+      <c r="I108" t="n">
+        <v>1</v>
+      </c>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
@@ -3092,12 +3384,16 @@
       </c>
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
-      <c r="I109" t="inlineStr"/>
+      <c r="I109" t="n">
+        <v>1</v>
+      </c>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
@@ -3117,12 +3413,16 @@
       </c>
       <c r="B110" t="inlineStr"/>
       <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
-      <c r="I110" t="inlineStr"/>
+      <c r="I110" t="n">
+        <v>1</v>
+      </c>
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
@@ -3165,12 +3465,16 @@
       </c>
       <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
-      <c r="I112" t="inlineStr"/>
+      <c r="I112" t="n">
+        <v>1</v>
+      </c>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
@@ -3188,12 +3492,16 @@
       </c>
       <c r="B113" t="inlineStr"/>
       <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr"/>
-      <c r="I113" t="inlineStr"/>
+      <c r="I113" t="n">
+        <v>1</v>
+      </c>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
@@ -3211,12 +3519,16 @@
       </c>
       <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
-      <c r="I114" t="inlineStr"/>
+      <c r="I114" t="n">
+        <v>1</v>
+      </c>
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
@@ -3234,12 +3546,16 @@
       </c>
       <c r="B115" t="inlineStr"/>
       <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr"/>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
-      <c r="I115" t="inlineStr"/>
+      <c r="I115" t="n">
+        <v>1</v>
+      </c>
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
@@ -3259,12 +3575,16 @@
       </c>
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr"/>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr"/>
+      <c r="I116" t="n">
+        <v>1</v>
+      </c>
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
@@ -3284,12 +3604,16 @@
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr"/>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr"/>
+      <c r="I117" t="n">
+        <v>1</v>
+      </c>
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr"/>
@@ -3307,7 +3631,9 @@
       </c>
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr"/>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
@@ -3332,12 +3658,16 @@
       </c>
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr"/>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr"/>
+      <c r="I119" t="n">
+        <v>1</v>
+      </c>
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
@@ -3357,12 +3687,16 @@
       </c>
       <c r="B120" t="inlineStr"/>
       <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr"/>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr"/>
+      <c r="I120" t="n">
+        <v>1</v>
+      </c>
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
@@ -3393,7 +3727,9 @@
       <c r="N121" t="inlineStr"/>
       <c r="O121" t="inlineStr"/>
       <c r="P121" t="inlineStr"/>
-      <c r="Q121" t="inlineStr"/>
+      <c r="Q121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3403,7 +3739,9 @@
       </c>
       <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr"/>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="n">
@@ -3412,7 +3750,9 @@
       <c r="H122" t="n">
         <v>1</v>
       </c>
-      <c r="I122" t="inlineStr"/>
+      <c r="I122" t="n">
+        <v>1</v>
+      </c>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
@@ -3430,12 +3770,16 @@
       </c>
       <c r="B123" t="inlineStr"/>
       <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr"/>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr"/>
-      <c r="I123" t="inlineStr"/>
+      <c r="I123" t="n">
+        <v>1</v>
+      </c>
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
@@ -3453,12 +3797,16 @@
       </c>
       <c r="B124" t="inlineStr"/>
       <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr"/>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
-      <c r="I124" t="inlineStr"/>
+      <c r="I124" t="n">
+        <v>1</v>
+      </c>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
@@ -3478,12 +3826,16 @@
       </c>
       <c r="B125" t="inlineStr"/>
       <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
-      <c r="I125" t="inlineStr"/>
+      <c r="I125" t="n">
+        <v>1</v>
+      </c>
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
@@ -3505,12 +3857,16 @@
       </c>
       <c r="B126" t="inlineStr"/>
       <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr"/>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="inlineStr"/>
-      <c r="I126" t="inlineStr"/>
+      <c r="I126" t="n">
+        <v>1</v>
+      </c>
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
@@ -3528,12 +3884,16 @@
       </c>
       <c r="B127" t="inlineStr"/>
       <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr"/>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr"/>
-      <c r="I127" t="inlineStr"/>
+      <c r="I127" t="n">
+        <v>1</v>
+      </c>
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
@@ -3551,12 +3911,16 @@
       </c>
       <c r="B128" t="inlineStr"/>
       <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr"/>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
-      <c r="I128" t="inlineStr"/>
+      <c r="I128" t="n">
+        <v>1</v>
+      </c>
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
@@ -3574,12 +3938,16 @@
       </c>
       <c r="B129" t="inlineStr"/>
       <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr"/>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr"/>
+      <c r="I129" t="n">
+        <v>1</v>
+      </c>
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
@@ -3597,12 +3965,16 @@
       </c>
       <c r="B130" t="inlineStr"/>
       <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr"/>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr"/>
+      <c r="I130" t="n">
+        <v>1</v>
+      </c>
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr"/>
@@ -3620,7 +3992,9 @@
       </c>
       <c r="B131" t="inlineStr"/>
       <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr"/>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="n">
@@ -3629,7 +4003,9 @@
       <c r="H131" t="n">
         <v>1</v>
       </c>
-      <c r="I131" t="inlineStr"/>
+      <c r="I131" t="n">
+        <v>1</v>
+      </c>
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr"/>
@@ -3647,12 +4023,16 @@
       </c>
       <c r="B132" t="inlineStr"/>
       <c r="C132" t="inlineStr"/>
-      <c r="D132" t="inlineStr"/>
+      <c r="D132" t="n">
+        <v>1</v>
+      </c>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
-      <c r="I132" t="inlineStr"/>
+      <c r="I132" t="n">
+        <v>1</v>
+      </c>
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr"/>
@@ -3670,12 +4050,16 @@
       </c>
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr"/>
-      <c r="D133" t="inlineStr"/>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
-      <c r="I133" t="inlineStr"/>
+      <c r="I133" t="n">
+        <v>1</v>
+      </c>
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr"/>
@@ -3693,7 +4077,9 @@
       </c>
       <c r="B134" t="inlineStr"/>
       <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr"/>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
       <c r="G134" t="n">
@@ -3702,7 +4088,9 @@
       <c r="H134" t="n">
         <v>1</v>
       </c>
-      <c r="I134" t="inlineStr"/>
+      <c r="I134" t="n">
+        <v>1</v>
+      </c>
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr"/>
@@ -3720,12 +4108,16 @@
       </c>
       <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr"/>
-      <c r="D135" t="inlineStr"/>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="inlineStr"/>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="inlineStr"/>
-      <c r="I135" t="inlineStr"/>
+      <c r="I135" t="n">
+        <v>1</v>
+      </c>
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
@@ -3743,12 +4135,16 @@
       </c>
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr"/>
-      <c r="D136" t="inlineStr"/>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
       <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr"/>
-      <c r="I136" t="inlineStr"/>
+      <c r="I136" t="n">
+        <v>1</v>
+      </c>
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
@@ -3766,12 +4162,16 @@
       </c>
       <c r="B137" t="inlineStr"/>
       <c r="C137" t="inlineStr"/>
-      <c r="D137" t="inlineStr"/>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="inlineStr"/>
-      <c r="I137" t="inlineStr"/>
+      <c r="I137" t="n">
+        <v>1</v>
+      </c>
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
@@ -3789,12 +4189,16 @@
       </c>
       <c r="B138" t="inlineStr"/>
       <c r="C138" t="inlineStr"/>
-      <c r="D138" t="inlineStr"/>
+      <c r="D138" t="n">
+        <v>1</v>
+      </c>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="inlineStr"/>
-      <c r="I138" t="inlineStr"/>
+      <c r="I138" t="n">
+        <v>1</v>
+      </c>
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
@@ -3811,7 +4215,9 @@
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>1</v>
+      </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
@@ -3835,12 +4241,16 @@
       </c>
       <c r="B140" t="inlineStr"/>
       <c r="C140" t="inlineStr"/>
-      <c r="D140" t="inlineStr"/>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
       <c r="E140" t="inlineStr"/>
       <c r="F140" t="inlineStr"/>
       <c r="G140" t="inlineStr"/>
       <c r="H140" t="inlineStr"/>
-      <c r="I140" t="inlineStr"/>
+      <c r="I140" t="n">
+        <v>1</v>
+      </c>
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
@@ -3862,12 +4272,16 @@
       </c>
       <c r="B141" t="inlineStr"/>
       <c r="C141" t="inlineStr"/>
-      <c r="D141" t="inlineStr"/>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr"/>
-      <c r="I141" t="inlineStr"/>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr"/>
@@ -3885,12 +4299,16 @@
       </c>
       <c r="B142" t="inlineStr"/>
       <c r="C142" t="inlineStr"/>
-      <c r="D142" t="inlineStr"/>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="inlineStr"/>
-      <c r="I142" t="inlineStr"/>
+      <c r="I142" t="n">
+        <v>1</v>
+      </c>
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
@@ -3908,12 +4326,16 @@
       </c>
       <c r="B143" t="inlineStr"/>
       <c r="C143" t="inlineStr"/>
-      <c r="D143" t="inlineStr"/>
+      <c r="D143" t="n">
+        <v>1</v>
+      </c>
       <c r="E143" t="inlineStr"/>
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="inlineStr"/>
-      <c r="I143" t="inlineStr"/>
+      <c r="I143" t="n">
+        <v>1</v>
+      </c>
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
@@ -3931,12 +4353,16 @@
       </c>
       <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr"/>
-      <c r="D144" t="inlineStr"/>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="inlineStr"/>
-      <c r="I144" t="inlineStr"/>
+      <c r="I144" t="n">
+        <v>1</v>
+      </c>
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
@@ -3967,7 +4393,9 @@
       <c r="N145" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="inlineStr"/>
-      <c r="Q145" t="inlineStr"/>
+      <c r="Q145" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3977,14 +4405,18 @@
       </c>
       <c r="B146" t="inlineStr"/>
       <c r="C146" t="inlineStr"/>
-      <c r="D146" t="inlineStr"/>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="inlineStr"/>
       <c r="G146" t="n">
         <v>1</v>
       </c>
       <c r="H146" t="inlineStr"/>
-      <c r="I146" t="inlineStr"/>
+      <c r="I146" t="n">
+        <v>1</v>
+      </c>
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
@@ -4002,7 +4434,9 @@
       </c>
       <c r="B147" t="inlineStr"/>
       <c r="C147" t="inlineStr"/>
-      <c r="D147" t="inlineStr"/>
+      <c r="D147" t="n">
+        <v>1</v>
+      </c>
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
@@ -4019,1792 +4453,6 @@
       <c r="P147" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
     </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>agrostis canina</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr"/>
-      <c r="C148" t="inlineStr"/>
-      <c r="D148" t="inlineStr"/>
-      <c r="E148" t="inlineStr"/>
-      <c r="F148" t="n">
-        <v>1</v>
-      </c>
-      <c r="G148" t="inlineStr"/>
-      <c r="H148" t="inlineStr"/>
-      <c r="I148" t="inlineStr"/>
-      <c r="J148" t="inlineStr"/>
-      <c r="K148" t="inlineStr"/>
-      <c r="L148" t="inlineStr"/>
-      <c r="M148" t="inlineStr"/>
-      <c r="N148" t="inlineStr"/>
-      <c r="O148" t="inlineStr"/>
-      <c r="P148" t="inlineStr"/>
-      <c r="Q148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>aira praecox</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr"/>
-      <c r="C149" t="inlineStr"/>
-      <c r="D149" t="inlineStr"/>
-      <c r="E149" t="inlineStr"/>
-      <c r="F149" t="inlineStr"/>
-      <c r="G149" t="inlineStr"/>
-      <c r="H149" t="inlineStr"/>
-      <c r="I149" t="inlineStr"/>
-      <c r="J149" t="inlineStr"/>
-      <c r="K149" t="inlineStr"/>
-      <c r="L149" t="inlineStr"/>
-      <c r="M149" t="inlineStr"/>
-      <c r="N149" t="inlineStr"/>
-      <c r="O149" t="inlineStr"/>
-      <c r="P149" t="inlineStr"/>
-      <c r="Q149" t="inlineStr"/>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>anisantha sterilis</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
-      <c r="D150" t="inlineStr"/>
-      <c r="E150" t="inlineStr"/>
-      <c r="F150" t="inlineStr"/>
-      <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
-      <c r="J150" t="inlineStr"/>
-      <c r="K150" t="inlineStr"/>
-      <c r="L150" t="inlineStr"/>
-      <c r="M150" t="inlineStr"/>
-      <c r="N150" t="inlineStr"/>
-      <c r="O150" t="inlineStr"/>
-      <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>arctium minus agg.</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr"/>
-      <c r="C151" t="inlineStr"/>
-      <c r="D151" t="inlineStr"/>
-      <c r="E151" t="inlineStr"/>
-      <c r="F151" t="inlineStr"/>
-      <c r="G151" t="inlineStr"/>
-      <c r="H151" t="inlineStr"/>
-      <c r="I151" t="inlineStr"/>
-      <c r="J151" t="inlineStr"/>
-      <c r="K151" t="inlineStr"/>
-      <c r="L151" t="inlineStr"/>
-      <c r="M151" t="inlineStr"/>
-      <c r="N151" t="inlineStr"/>
-      <c r="O151" t="inlineStr"/>
-      <c r="P151" t="inlineStr"/>
-      <c r="Q151" t="inlineStr"/>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>blackstonia perfoliata</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr"/>
-      <c r="C152" t="inlineStr"/>
-      <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr"/>
-      <c r="F152" t="inlineStr"/>
-      <c r="G152" t="inlineStr"/>
-      <c r="H152" t="inlineStr"/>
-      <c r="I152" t="inlineStr"/>
-      <c r="J152" t="inlineStr"/>
-      <c r="K152" t="inlineStr"/>
-      <c r="L152" t="inlineStr"/>
-      <c r="M152" t="inlineStr"/>
-      <c r="N152" t="inlineStr"/>
-      <c r="O152" t="inlineStr"/>
-      <c r="P152" t="inlineStr"/>
-      <c r="Q152" t="inlineStr"/>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>bryonia dioica</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-      <c r="D153" t="inlineStr"/>
-      <c r="E153" t="inlineStr"/>
-      <c r="F153" t="inlineStr"/>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
-      <c r="I153" t="inlineStr"/>
-      <c r="J153" t="inlineStr"/>
-      <c r="K153" t="inlineStr"/>
-      <c r="L153" t="inlineStr"/>
-      <c r="M153" t="inlineStr"/>
-      <c r="N153" t="inlineStr"/>
-      <c r="O153" t="inlineStr"/>
-      <c r="P153" t="inlineStr"/>
-      <c r="Q153" t="inlineStr"/>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>chamerion angustifolium</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr"/>
-      <c r="C154" t="inlineStr"/>
-      <c r="D154" t="inlineStr"/>
-      <c r="E154" t="inlineStr"/>
-      <c r="F154" t="inlineStr"/>
-      <c r="G154" t="inlineStr"/>
-      <c r="H154" t="inlineStr"/>
-      <c r="I154" t="inlineStr"/>
-      <c r="J154" t="inlineStr"/>
-      <c r="K154" t="inlineStr"/>
-      <c r="L154" t="inlineStr"/>
-      <c r="M154" t="inlineStr"/>
-      <c r="N154" t="inlineStr"/>
-      <c r="O154" t="inlineStr"/>
-      <c r="P154" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q154" t="inlineStr"/>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>crataegus monogyna (c)</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
-      <c r="D155" t="inlineStr"/>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr"/>
-      <c r="G155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
-      <c r="I155" t="inlineStr"/>
-      <c r="J155" t="inlineStr"/>
-      <c r="K155" t="inlineStr"/>
-      <c r="L155" t="inlineStr"/>
-      <c r="M155" t="inlineStr"/>
-      <c r="N155" t="inlineStr"/>
-      <c r="O155" t="inlineStr"/>
-      <c r="P155" t="inlineStr"/>
-      <c r="Q155" t="inlineStr"/>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>dryopteris filix-mas</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
-      <c r="F156" t="inlineStr"/>
-      <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="inlineStr"/>
-      <c r="J156" t="inlineStr"/>
-      <c r="K156" t="inlineStr"/>
-      <c r="L156" t="inlineStr"/>
-      <c r="M156" t="inlineStr"/>
-      <c r="N156" t="inlineStr"/>
-      <c r="O156" t="inlineStr"/>
-      <c r="P156" t="inlineStr"/>
-      <c r="Q156" t="inlineStr"/>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>epilobium ciliatum</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
-      <c r="D157" t="inlineStr"/>
-      <c r="E157" t="inlineStr"/>
-      <c r="F157" t="inlineStr"/>
-      <c r="G157" t="inlineStr"/>
-      <c r="H157" t="inlineStr"/>
-      <c r="I157" t="inlineStr"/>
-      <c r="J157" t="inlineStr"/>
-      <c r="K157" t="inlineStr"/>
-      <c r="L157" t="inlineStr"/>
-      <c r="M157" t="inlineStr"/>
-      <c r="N157" t="inlineStr"/>
-      <c r="O157" t="inlineStr"/>
-      <c r="P157" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q157" t="inlineStr"/>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>epilobium parviflorum</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr"/>
-      <c r="C158" t="inlineStr"/>
-      <c r="D158" t="inlineStr"/>
-      <c r="E158" t="inlineStr"/>
-      <c r="F158" t="inlineStr"/>
-      <c r="G158" t="inlineStr"/>
-      <c r="H158" t="inlineStr"/>
-      <c r="I158" t="inlineStr"/>
-      <c r="J158" t="inlineStr"/>
-      <c r="K158" t="inlineStr"/>
-      <c r="L158" t="inlineStr"/>
-      <c r="M158" t="inlineStr"/>
-      <c r="N158" t="inlineStr"/>
-      <c r="O158" t="inlineStr"/>
-      <c r="P158" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q158" t="inlineStr"/>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>euphrasia officinalis agg.</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr"/>
-      <c r="C159" t="inlineStr"/>
-      <c r="D159" t="inlineStr"/>
-      <c r="E159" t="inlineStr"/>
-      <c r="F159" t="inlineStr"/>
-      <c r="G159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
-      <c r="I159" t="inlineStr"/>
-      <c r="J159" t="inlineStr"/>
-      <c r="K159" t="inlineStr"/>
-      <c r="L159" t="inlineStr"/>
-      <c r="M159" t="inlineStr"/>
-      <c r="N159" t="inlineStr"/>
-      <c r="O159" t="inlineStr"/>
-      <c r="P159" t="inlineStr"/>
-      <c r="Q159" t="inlineStr"/>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>fissidens</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-      <c r="D160" t="inlineStr"/>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr"/>
-      <c r="G160" t="inlineStr"/>
-      <c r="H160" t="inlineStr"/>
-      <c r="I160" t="inlineStr"/>
-      <c r="J160" t="inlineStr"/>
-      <c r="K160" t="inlineStr"/>
-      <c r="L160" t="inlineStr"/>
-      <c r="M160" t="inlineStr"/>
-      <c r="N160" t="inlineStr"/>
-      <c r="O160" t="inlineStr"/>
-      <c r="P160" t="inlineStr"/>
-      <c r="Q160" t="inlineStr"/>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>geranium dissectum</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
-      <c r="D161" t="inlineStr"/>
-      <c r="E161" t="inlineStr"/>
-      <c r="F161" t="inlineStr"/>
-      <c r="G161" t="inlineStr"/>
-      <c r="H161" t="inlineStr"/>
-      <c r="I161" t="inlineStr"/>
-      <c r="J161" t="inlineStr"/>
-      <c r="K161" t="inlineStr"/>
-      <c r="L161" t="inlineStr"/>
-      <c r="M161" t="inlineStr"/>
-      <c r="N161" t="inlineStr"/>
-      <c r="O161" t="inlineStr"/>
-      <c r="P161" t="inlineStr"/>
-      <c r="Q161" t="inlineStr"/>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>helictotrichon pubescens</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr"/>
-      <c r="C162" t="inlineStr"/>
-      <c r="D162" t="inlineStr"/>
-      <c r="E162" t="inlineStr"/>
-      <c r="F162" t="inlineStr"/>
-      <c r="G162" t="inlineStr"/>
-      <c r="H162" t="inlineStr"/>
-      <c r="I162" t="inlineStr"/>
-      <c r="J162" t="inlineStr"/>
-      <c r="K162" t="inlineStr"/>
-      <c r="L162" t="inlineStr"/>
-      <c r="M162" t="inlineStr"/>
-      <c r="N162" t="inlineStr"/>
-      <c r="O162" t="inlineStr"/>
-      <c r="P162" t="inlineStr"/>
-      <c r="Q162" t="inlineStr"/>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>hypnum cupressiforme</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr"/>
-      <c r="D163" t="inlineStr"/>
-      <c r="E163" t="inlineStr"/>
-      <c r="F163" t="inlineStr"/>
-      <c r="G163" t="inlineStr"/>
-      <c r="H163" t="inlineStr"/>
-      <c r="I163" t="inlineStr"/>
-      <c r="J163" t="inlineStr"/>
-      <c r="K163" t="inlineStr"/>
-      <c r="L163" t="inlineStr"/>
-      <c r="M163" t="inlineStr"/>
-      <c r="N163" t="inlineStr"/>
-      <c r="O163" t="inlineStr"/>
-      <c r="P163" t="inlineStr"/>
-      <c r="Q163" t="inlineStr"/>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>lolium perenne</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr"/>
-      <c r="D164" t="inlineStr"/>
-      <c r="E164" t="inlineStr"/>
-      <c r="F164" t="inlineStr"/>
-      <c r="G164" t="inlineStr"/>
-      <c r="H164" t="inlineStr"/>
-      <c r="I164" t="inlineStr"/>
-      <c r="J164" t="inlineStr"/>
-      <c r="K164" t="inlineStr"/>
-      <c r="L164" t="inlineStr"/>
-      <c r="M164" t="inlineStr"/>
-      <c r="N164" t="inlineStr"/>
-      <c r="O164" t="inlineStr"/>
-      <c r="P164" t="inlineStr"/>
-      <c r="Q164" t="inlineStr"/>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>luzula multiflora</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr"/>
-      <c r="C165" t="inlineStr"/>
-      <c r="D165" t="inlineStr"/>
-      <c r="E165" t="inlineStr"/>
-      <c r="F165" t="inlineStr"/>
-      <c r="G165" t="inlineStr"/>
-      <c r="H165" t="inlineStr"/>
-      <c r="I165" t="inlineStr"/>
-      <c r="J165" t="inlineStr"/>
-      <c r="K165" t="inlineStr"/>
-      <c r="L165" t="inlineStr"/>
-      <c r="M165" t="inlineStr"/>
-      <c r="N165" t="inlineStr"/>
-      <c r="O165" t="inlineStr"/>
-      <c r="P165" t="inlineStr"/>
-      <c r="Q165" t="inlineStr"/>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>malus sylvestris (seedling)</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-      <c r="D166" t="inlineStr"/>
-      <c r="E166" t="inlineStr"/>
-      <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="inlineStr"/>
-      <c r="J166" t="inlineStr"/>
-      <c r="K166" t="inlineStr"/>
-      <c r="L166" t="inlineStr"/>
-      <c r="M166" t="inlineStr"/>
-      <c r="N166" t="inlineStr"/>
-      <c r="O166" t="inlineStr"/>
-      <c r="P166" t="inlineStr"/>
-      <c r="Q166" t="inlineStr"/>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>myosotis arvensis</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr"/>
-      <c r="C167" t="inlineStr"/>
-      <c r="D167" t="inlineStr"/>
-      <c r="E167" t="inlineStr"/>
-      <c r="F167" t="inlineStr"/>
-      <c r="G167" t="inlineStr"/>
-      <c r="H167" t="inlineStr"/>
-      <c r="I167" t="inlineStr"/>
-      <c r="J167" t="inlineStr"/>
-      <c r="K167" t="inlineStr"/>
-      <c r="L167" t="inlineStr"/>
-      <c r="M167" t="inlineStr"/>
-      <c r="N167" t="inlineStr"/>
-      <c r="O167" t="inlineStr"/>
-      <c r="P167" t="inlineStr"/>
-      <c r="Q167" t="inlineStr"/>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>myosotis discolor</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
-      <c r="D168" t="inlineStr"/>
-      <c r="E168" t="inlineStr"/>
-      <c r="F168" t="inlineStr"/>
-      <c r="G168" t="inlineStr"/>
-      <c r="H168" t="inlineStr"/>
-      <c r="I168" t="inlineStr"/>
-      <c r="J168" t="inlineStr"/>
-      <c r="K168" t="inlineStr"/>
-      <c r="L168" t="inlineStr"/>
-      <c r="M168" t="inlineStr"/>
-      <c r="N168" t="inlineStr"/>
-      <c r="O168" t="inlineStr"/>
-      <c r="P168" t="inlineStr"/>
-      <c r="Q168" t="inlineStr"/>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>poa</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr"/>
-      <c r="C169" t="inlineStr"/>
-      <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr"/>
-      <c r="F169" t="inlineStr"/>
-      <c r="G169" t="inlineStr"/>
-      <c r="H169" t="inlineStr"/>
-      <c r="I169" t="inlineStr"/>
-      <c r="J169" t="inlineStr"/>
-      <c r="K169" t="inlineStr"/>
-      <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr"/>
-      <c r="N169" t="inlineStr"/>
-      <c r="O169" t="inlineStr"/>
-      <c r="P169" t="inlineStr"/>
-      <c r="Q169" t="inlineStr"/>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>poa annua</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-      <c r="D170" t="inlineStr"/>
-      <c r="E170" t="inlineStr"/>
-      <c r="F170" t="inlineStr"/>
-      <c r="G170" t="inlineStr"/>
-      <c r="H170" t="inlineStr"/>
-      <c r="I170" t="inlineStr"/>
-      <c r="J170" t="inlineStr"/>
-      <c r="K170" t="inlineStr"/>
-      <c r="L170" t="inlineStr"/>
-      <c r="M170" t="inlineStr"/>
-      <c r="N170" t="inlineStr"/>
-      <c r="O170" t="inlineStr"/>
-      <c r="P170" t="inlineStr"/>
-      <c r="Q170" t="inlineStr"/>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>poa trivialis</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr"/>
-      <c r="C171" t="inlineStr"/>
-      <c r="D171" t="inlineStr"/>
-      <c r="E171" t="inlineStr"/>
-      <c r="F171" t="inlineStr"/>
-      <c r="G171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
-      <c r="I171" t="inlineStr"/>
-      <c r="J171" t="inlineStr"/>
-      <c r="K171" t="inlineStr"/>
-      <c r="L171" t="inlineStr"/>
-      <c r="M171" t="inlineStr"/>
-      <c r="N171" t="inlineStr"/>
-      <c r="O171" t="inlineStr"/>
-      <c r="P171" t="inlineStr"/>
-      <c r="Q171" t="inlineStr"/>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>polygala serpyllifolia</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr"/>
-      <c r="C172" t="inlineStr"/>
-      <c r="D172" t="inlineStr"/>
-      <c r="E172" t="inlineStr"/>
-      <c r="F172" t="inlineStr"/>
-      <c r="G172" t="n">
-        <v>1</v>
-      </c>
-      <c r="H172" t="n">
-        <v>1</v>
-      </c>
-      <c r="I172" t="n">
-        <v>1</v>
-      </c>
-      <c r="J172" t="inlineStr"/>
-      <c r="K172" t="inlineStr"/>
-      <c r="L172" t="inlineStr"/>
-      <c r="M172" t="inlineStr"/>
-      <c r="N172" t="inlineStr"/>
-      <c r="O172" t="inlineStr"/>
-      <c r="P172" t="inlineStr"/>
-      <c r="Q172" t="inlineStr"/>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>prunus padus (g)</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr"/>
-      <c r="C173" t="inlineStr"/>
-      <c r="D173" t="inlineStr"/>
-      <c r="E173" t="inlineStr"/>
-      <c r="F173" t="inlineStr"/>
-      <c r="G173" t="inlineStr"/>
-      <c r="H173" t="inlineStr"/>
-      <c r="I173" t="inlineStr"/>
-      <c r="J173" t="inlineStr"/>
-      <c r="K173" t="inlineStr"/>
-      <c r="L173" t="inlineStr"/>
-      <c r="M173" t="inlineStr"/>
-      <c r="N173" t="inlineStr"/>
-      <c r="O173" t="inlineStr"/>
-      <c r="P173" t="inlineStr"/>
-      <c r="Q173" t="inlineStr"/>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>prunus spinosa (s)</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr"/>
-      <c r="D174" t="inlineStr"/>
-      <c r="E174" t="inlineStr"/>
-      <c r="F174" t="inlineStr"/>
-      <c r="G174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
-      <c r="I174" t="inlineStr"/>
-      <c r="J174" t="inlineStr"/>
-      <c r="K174" t="inlineStr"/>
-      <c r="L174" t="inlineStr"/>
-      <c r="M174" t="inlineStr"/>
-      <c r="N174" t="inlineStr"/>
-      <c r="O174" t="inlineStr"/>
-      <c r="P174" t="inlineStr"/>
-      <c r="Q174" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>reseda lutea</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
-      <c r="D175" t="inlineStr"/>
-      <c r="E175" t="inlineStr"/>
-      <c r="F175" t="inlineStr"/>
-      <c r="G175" t="inlineStr"/>
-      <c r="H175" t="inlineStr"/>
-      <c r="I175" t="inlineStr"/>
-      <c r="J175" t="inlineStr"/>
-      <c r="K175" t="inlineStr"/>
-      <c r="L175" t="inlineStr"/>
-      <c r="M175" t="inlineStr"/>
-      <c r="N175" t="inlineStr"/>
-      <c r="O175" t="inlineStr"/>
-      <c r="P175" t="inlineStr"/>
-      <c r="Q175" t="inlineStr"/>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>rhizomnium punctatum</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr"/>
-      <c r="C176" t="inlineStr"/>
-      <c r="D176" t="inlineStr"/>
-      <c r="E176" t="inlineStr"/>
-      <c r="F176" t="inlineStr"/>
-      <c r="G176" t="inlineStr"/>
-      <c r="H176" t="inlineStr"/>
-      <c r="I176" t="inlineStr"/>
-      <c r="J176" t="inlineStr"/>
-      <c r="K176" t="inlineStr"/>
-      <c r="L176" t="inlineStr"/>
-      <c r="M176" t="inlineStr"/>
-      <c r="N176" t="inlineStr"/>
-      <c r="O176" t="inlineStr"/>
-      <c r="P176" t="inlineStr"/>
-      <c r="Q176" t="inlineStr"/>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>rhytidiadelphus squarrosus</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr"/>
-      <c r="C177" t="inlineStr"/>
-      <c r="D177" t="inlineStr"/>
-      <c r="E177" t="inlineStr"/>
-      <c r="F177" t="inlineStr"/>
-      <c r="G177" t="inlineStr"/>
-      <c r="H177" t="inlineStr"/>
-      <c r="I177" t="inlineStr"/>
-      <c r="J177" t="inlineStr"/>
-      <c r="K177" t="inlineStr"/>
-      <c r="L177" t="inlineStr"/>
-      <c r="M177" t="inlineStr"/>
-      <c r="N177" t="inlineStr"/>
-      <c r="O177" t="inlineStr"/>
-      <c r="P177" t="inlineStr"/>
-      <c r="Q177" t="inlineStr"/>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>rosa arvensis</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr"/>
-      <c r="C178" t="inlineStr"/>
-      <c r="D178" t="inlineStr"/>
-      <c r="E178" t="inlineStr"/>
-      <c r="F178" t="inlineStr"/>
-      <c r="G178" t="inlineStr"/>
-      <c r="H178" t="inlineStr"/>
-      <c r="I178" t="inlineStr"/>
-      <c r="J178" t="inlineStr"/>
-      <c r="K178" t="inlineStr"/>
-      <c r="L178" t="inlineStr"/>
-      <c r="M178" t="inlineStr"/>
-      <c r="N178" t="inlineStr"/>
-      <c r="O178" t="inlineStr"/>
-      <c r="P178" t="inlineStr"/>
-      <c r="Q178" t="inlineStr"/>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>rosa spinosissima</t>
-        </is>
-      </c>
-      <c r="B179" t="inlineStr"/>
-      <c r="C179" t="inlineStr"/>
-      <c r="D179" t="inlineStr"/>
-      <c r="E179" t="inlineStr"/>
-      <c r="F179" t="inlineStr"/>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" t="inlineStr"/>
-      <c r="I179" t="inlineStr"/>
-      <c r="J179" t="inlineStr"/>
-      <c r="K179" t="inlineStr"/>
-      <c r="L179" t="inlineStr"/>
-      <c r="M179" t="inlineStr"/>
-      <c r="N179" t="inlineStr"/>
-      <c r="O179" t="inlineStr"/>
-      <c r="P179" t="inlineStr"/>
-      <c r="Q179" t="inlineStr"/>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>sherardia arvensis</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr"/>
-      <c r="C180" t="inlineStr"/>
-      <c r="D180" t="inlineStr"/>
-      <c r="E180" t="inlineStr"/>
-      <c r="F180" t="inlineStr"/>
-      <c r="G180" t="inlineStr"/>
-      <c r="H180" t="inlineStr"/>
-      <c r="I180" t="inlineStr"/>
-      <c r="J180" t="inlineStr"/>
-      <c r="K180" t="inlineStr"/>
-      <c r="L180" t="inlineStr"/>
-      <c r="M180" t="inlineStr"/>
-      <c r="N180" t="inlineStr"/>
-      <c r="O180" t="inlineStr"/>
-      <c r="P180" t="inlineStr"/>
-      <c r="Q180" t="inlineStr"/>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>sonchus asper</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr"/>
-      <c r="C181" t="inlineStr"/>
-      <c r="D181" t="inlineStr"/>
-      <c r="E181" t="inlineStr"/>
-      <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
-      <c r="I181" t="inlineStr"/>
-      <c r="J181" t="inlineStr"/>
-      <c r="K181" t="inlineStr"/>
-      <c r="L181" t="inlineStr"/>
-      <c r="M181" t="inlineStr"/>
-      <c r="N181" t="inlineStr"/>
-      <c r="O181" t="inlineStr"/>
-      <c r="P181" t="inlineStr"/>
-      <c r="Q181" t="inlineStr"/>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>taraxacum agg.</t>
-        </is>
-      </c>
-      <c r="B182" t="inlineStr"/>
-      <c r="C182" t="inlineStr"/>
-      <c r="D182" t="inlineStr"/>
-      <c r="E182" t="inlineStr"/>
-      <c r="F182" t="inlineStr"/>
-      <c r="G182" t="inlineStr"/>
-      <c r="H182" t="inlineStr"/>
-      <c r="I182" t="inlineStr"/>
-      <c r="J182" t="inlineStr"/>
-      <c r="K182" t="inlineStr"/>
-      <c r="L182" t="inlineStr"/>
-      <c r="M182" t="inlineStr"/>
-      <c r="N182" t="inlineStr"/>
-      <c r="O182" t="inlineStr"/>
-      <c r="P182" t="inlineStr"/>
-      <c r="Q182" t="inlineStr"/>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>thymus pulegioides</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr"/>
-      <c r="C183" t="inlineStr"/>
-      <c r="D183" t="inlineStr"/>
-      <c r="E183" t="inlineStr"/>
-      <c r="F183" t="inlineStr"/>
-      <c r="G183" t="n">
-        <v>1</v>
-      </c>
-      <c r="H183" t="n">
-        <v>1</v>
-      </c>
-      <c r="I183" t="inlineStr"/>
-      <c r="J183" t="inlineStr"/>
-      <c r="K183" t="inlineStr"/>
-      <c r="L183" t="inlineStr"/>
-      <c r="M183" t="inlineStr"/>
-      <c r="N183" t="inlineStr"/>
-      <c r="O183" t="inlineStr"/>
-      <c r="P183" t="inlineStr"/>
-      <c r="Q183" t="inlineStr"/>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>trifolium dubium</t>
-        </is>
-      </c>
-      <c r="B184" t="inlineStr"/>
-      <c r="C184" t="inlineStr"/>
-      <c r="D184" t="inlineStr"/>
-      <c r="E184" t="inlineStr"/>
-      <c r="F184" t="inlineStr"/>
-      <c r="G184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
-      <c r="I184" t="inlineStr"/>
-      <c r="J184" t="inlineStr"/>
-      <c r="K184" t="inlineStr"/>
-      <c r="L184" t="inlineStr"/>
-      <c r="M184" t="inlineStr"/>
-      <c r="N184" t="inlineStr"/>
-      <c r="O184" t="inlineStr"/>
-      <c r="P184" t="inlineStr"/>
-      <c r="Q184" t="inlineStr"/>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>ulex europaeus (s)</t>
-        </is>
-      </c>
-      <c r="B185" t="inlineStr"/>
-      <c r="C185" t="inlineStr"/>
-      <c r="D185" t="inlineStr"/>
-      <c r="E185" t="inlineStr"/>
-      <c r="F185" t="inlineStr"/>
-      <c r="G185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
-      <c r="I185" t="inlineStr"/>
-      <c r="J185" t="inlineStr"/>
-      <c r="K185" t="inlineStr"/>
-      <c r="L185" t="inlineStr"/>
-      <c r="M185" t="inlineStr"/>
-      <c r="N185" t="inlineStr"/>
-      <c r="O185" t="inlineStr"/>
-      <c r="P185" t="inlineStr"/>
-      <c r="Q185" t="inlineStr"/>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>veronica serpyllifolia sl.</t>
-        </is>
-      </c>
-      <c r="B186" t="inlineStr"/>
-      <c r="C186" t="inlineStr"/>
-      <c r="D186" t="inlineStr"/>
-      <c r="E186" t="inlineStr"/>
-      <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
-      <c r="I186" t="inlineStr"/>
-      <c r="J186" t="inlineStr"/>
-      <c r="K186" t="inlineStr"/>
-      <c r="L186" t="inlineStr"/>
-      <c r="M186" t="inlineStr"/>
-      <c r="N186" t="inlineStr"/>
-      <c r="O186" t="inlineStr"/>
-      <c r="P186" t="inlineStr"/>
-      <c r="Q186" t="inlineStr"/>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>vulpia bromoides</t>
-        </is>
-      </c>
-      <c r="B187" t="inlineStr"/>
-      <c r="C187" t="inlineStr"/>
-      <c r="D187" t="inlineStr"/>
-      <c r="E187" t="inlineStr"/>
-      <c r="F187" t="inlineStr"/>
-      <c r="G187" t="inlineStr"/>
-      <c r="H187" t="inlineStr"/>
-      <c r="I187" t="inlineStr"/>
-      <c r="J187" t="inlineStr"/>
-      <c r="K187" t="inlineStr"/>
-      <c r="L187" t="inlineStr"/>
-      <c r="M187" t="inlineStr"/>
-      <c r="N187" t="inlineStr"/>
-      <c r="O187" t="inlineStr"/>
-      <c r="P187" t="inlineStr"/>
-      <c r="Q187" t="inlineStr"/>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>agrimonia</t>
-        </is>
-      </c>
-      <c r="B188" t="inlineStr"/>
-      <c r="C188" t="inlineStr"/>
-      <c r="D188" t="inlineStr"/>
-      <c r="E188" t="inlineStr"/>
-      <c r="F188" t="inlineStr"/>
-      <c r="G188" t="inlineStr"/>
-      <c r="H188" t="inlineStr"/>
-      <c r="I188" t="inlineStr"/>
-      <c r="J188" t="inlineStr"/>
-      <c r="K188" t="inlineStr"/>
-      <c r="L188" t="inlineStr"/>
-      <c r="M188" t="inlineStr"/>
-      <c r="N188" t="inlineStr"/>
-      <c r="O188" t="inlineStr"/>
-      <c r="P188" t="inlineStr"/>
-      <c r="Q188" t="inlineStr"/>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>brachythecium</t>
-        </is>
-      </c>
-      <c r="B189" t="inlineStr"/>
-      <c r="C189" t="inlineStr"/>
-      <c r="D189" t="inlineStr"/>
-      <c r="E189" t="inlineStr"/>
-      <c r="F189" t="inlineStr"/>
-      <c r="G189" t="inlineStr"/>
-      <c r="H189" t="inlineStr"/>
-      <c r="I189" t="inlineStr"/>
-      <c r="J189" t="inlineStr"/>
-      <c r="K189" t="inlineStr"/>
-      <c r="L189" t="inlineStr"/>
-      <c r="M189" t="inlineStr"/>
-      <c r="N189" t="inlineStr"/>
-      <c r="O189" t="inlineStr"/>
-      <c r="P189" t="inlineStr"/>
-      <c r="Q189" t="inlineStr"/>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>bromopsis ramosa</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr"/>
-      <c r="C190" t="inlineStr"/>
-      <c r="D190" t="inlineStr"/>
-      <c r="E190" t="inlineStr"/>
-      <c r="F190" t="inlineStr"/>
-      <c r="G190" t="inlineStr"/>
-      <c r="H190" t="inlineStr"/>
-      <c r="I190" t="inlineStr"/>
-      <c r="J190" t="inlineStr"/>
-      <c r="K190" t="inlineStr"/>
-      <c r="L190" t="inlineStr"/>
-      <c r="M190" t="inlineStr"/>
-      <c r="N190" t="inlineStr"/>
-      <c r="O190" t="inlineStr"/>
-      <c r="P190" t="inlineStr"/>
-      <c r="Q190" t="inlineStr"/>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>centaurea</t>
-        </is>
-      </c>
-      <c r="B191" t="inlineStr"/>
-      <c r="C191" t="inlineStr"/>
-      <c r="D191" t="inlineStr"/>
-      <c r="E191" t="inlineStr"/>
-      <c r="F191" t="inlineStr"/>
-      <c r="G191" t="inlineStr"/>
-      <c r="H191" t="inlineStr"/>
-      <c r="I191" t="inlineStr"/>
-      <c r="J191" t="inlineStr"/>
-      <c r="K191" t="inlineStr"/>
-      <c r="L191" t="inlineStr"/>
-      <c r="M191" t="inlineStr"/>
-      <c r="N191" t="inlineStr"/>
-      <c r="O191" t="inlineStr"/>
-      <c r="P191" t="inlineStr"/>
-      <c r="Q191" t="inlineStr"/>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>cladonia furcata</t>
-        </is>
-      </c>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
-      <c r="D192" t="inlineStr"/>
-      <c r="E192" t="inlineStr"/>
-      <c r="F192" t="inlineStr"/>
-      <c r="G192" t="inlineStr"/>
-      <c r="H192" t="inlineStr"/>
-      <c r="I192" t="inlineStr"/>
-      <c r="J192" t="inlineStr"/>
-      <c r="K192" t="inlineStr"/>
-      <c r="L192" t="inlineStr"/>
-      <c r="M192" t="inlineStr"/>
-      <c r="N192" t="inlineStr"/>
-      <c r="O192" t="inlineStr"/>
-      <c r="P192" t="inlineStr"/>
-      <c r="Q192" t="inlineStr"/>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>crepis vesicaria</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
-      <c r="D193" t="inlineStr"/>
-      <c r="E193" t="inlineStr"/>
-      <c r="F193" t="inlineStr"/>
-      <c r="G193" t="inlineStr"/>
-      <c r="H193" t="inlineStr"/>
-      <c r="I193" t="inlineStr"/>
-      <c r="J193" t="inlineStr"/>
-      <c r="K193" t="inlineStr"/>
-      <c r="L193" t="inlineStr"/>
-      <c r="M193" t="inlineStr"/>
-      <c r="N193" t="inlineStr"/>
-      <c r="O193" t="inlineStr"/>
-      <c r="P193" t="inlineStr"/>
-      <c r="Q193" t="inlineStr"/>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>cruciata laevipes</t>
-        </is>
-      </c>
-      <c r="B194" t="inlineStr"/>
-      <c r="C194" t="inlineStr"/>
-      <c r="D194" t="inlineStr"/>
-      <c r="E194" t="inlineStr"/>
-      <c r="F194" t="inlineStr"/>
-      <c r="G194" t="inlineStr"/>
-      <c r="H194" t="inlineStr"/>
-      <c r="I194" t="inlineStr"/>
-      <c r="J194" t="inlineStr"/>
-      <c r="K194" t="inlineStr"/>
-      <c r="L194" t="inlineStr"/>
-      <c r="M194" t="inlineStr"/>
-      <c r="N194" t="inlineStr"/>
-      <c r="O194" t="inlineStr"/>
-      <c r="P194" t="inlineStr"/>
-      <c r="Q194" t="inlineStr"/>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>cynoglossum</t>
-        </is>
-      </c>
-      <c r="B195" t="inlineStr"/>
-      <c r="C195" t="inlineStr"/>
-      <c r="D195" t="inlineStr"/>
-      <c r="E195" t="inlineStr"/>
-      <c r="F195" t="inlineStr"/>
-      <c r="G195" t="inlineStr"/>
-      <c r="H195" t="inlineStr"/>
-      <c r="I195" t="inlineStr"/>
-      <c r="J195" t="inlineStr"/>
-      <c r="K195" t="inlineStr"/>
-      <c r="L195" t="inlineStr"/>
-      <c r="M195" t="inlineStr"/>
-      <c r="N195" t="inlineStr"/>
-      <c r="O195" t="inlineStr"/>
-      <c r="P195" t="inlineStr"/>
-      <c r="Q195" t="inlineStr"/>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>daucus carota</t>
-        </is>
-      </c>
-      <c r="B196" t="inlineStr"/>
-      <c r="C196" t="inlineStr"/>
-      <c r="D196" t="inlineStr"/>
-      <c r="E196" t="inlineStr"/>
-      <c r="F196" t="inlineStr"/>
-      <c r="G196" t="inlineStr"/>
-      <c r="H196" t="inlineStr"/>
-      <c r="I196" t="inlineStr"/>
-      <c r="J196" t="inlineStr"/>
-      <c r="K196" t="inlineStr"/>
-      <c r="L196" t="inlineStr"/>
-      <c r="M196" t="inlineStr"/>
-      <c r="N196" t="inlineStr"/>
-      <c r="O196" t="inlineStr"/>
-      <c r="P196" t="inlineStr"/>
-      <c r="Q196" t="inlineStr"/>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>deschampsia flexuosa</t>
-        </is>
-      </c>
-      <c r="B197" t="inlineStr"/>
-      <c r="C197" t="inlineStr"/>
-      <c r="D197" t="inlineStr"/>
-      <c r="E197" t="inlineStr"/>
-      <c r="F197" t="n">
-        <v>1</v>
-      </c>
-      <c r="G197" t="inlineStr"/>
-      <c r="H197" t="inlineStr"/>
-      <c r="I197" t="inlineStr"/>
-      <c r="J197" t="inlineStr"/>
-      <c r="K197" t="inlineStr"/>
-      <c r="L197" t="inlineStr"/>
-      <c r="M197" t="inlineStr"/>
-      <c r="N197" t="inlineStr"/>
-      <c r="O197" t="inlineStr"/>
-      <c r="P197" t="inlineStr"/>
-      <c r="Q197" t="inlineStr"/>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>euonymus europaeus (g)</t>
-        </is>
-      </c>
-      <c r="B198" t="inlineStr"/>
-      <c r="C198" t="inlineStr"/>
-      <c r="D198" t="inlineStr"/>
-      <c r="E198" t="inlineStr"/>
-      <c r="F198" t="inlineStr"/>
-      <c r="G198" t="inlineStr"/>
-      <c r="H198" t="inlineStr"/>
-      <c r="I198" t="inlineStr"/>
-      <c r="J198" t="inlineStr"/>
-      <c r="K198" t="inlineStr"/>
-      <c r="L198" t="inlineStr"/>
-      <c r="M198" t="inlineStr"/>
-      <c r="N198" t="inlineStr"/>
-      <c r="O198" t="inlineStr"/>
-      <c r="P198" t="inlineStr"/>
-      <c r="Q198" t="inlineStr"/>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>galium mollugo</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr"/>
-      <c r="C199" t="inlineStr"/>
-      <c r="D199" t="inlineStr"/>
-      <c r="E199" t="inlineStr"/>
-      <c r="F199" t="inlineStr"/>
-      <c r="G199" t="inlineStr"/>
-      <c r="H199" t="inlineStr"/>
-      <c r="I199" t="inlineStr"/>
-      <c r="J199" t="inlineStr"/>
-      <c r="K199" t="inlineStr"/>
-      <c r="L199" t="inlineStr"/>
-      <c r="M199" t="inlineStr"/>
-      <c r="N199" t="inlineStr"/>
-      <c r="O199" t="inlineStr"/>
-      <c r="P199" t="inlineStr"/>
-      <c r="Q199" t="inlineStr"/>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>galium mollugo subsp. erectum</t>
-        </is>
-      </c>
-      <c r="B200" t="inlineStr"/>
-      <c r="C200" t="inlineStr"/>
-      <c r="D200" t="inlineStr"/>
-      <c r="E200" t="inlineStr"/>
-      <c r="F200" t="inlineStr"/>
-      <c r="G200" t="inlineStr"/>
-      <c r="H200" t="inlineStr"/>
-      <c r="I200" t="inlineStr"/>
-      <c r="J200" t="inlineStr"/>
-      <c r="K200" t="inlineStr"/>
-      <c r="L200" t="inlineStr"/>
-      <c r="M200" t="inlineStr"/>
-      <c r="N200" t="inlineStr"/>
-      <c r="O200" t="inlineStr"/>
-      <c r="P200" t="inlineStr"/>
-      <c r="Q200" t="inlineStr"/>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>heracleum sphondylium</t>
-        </is>
-      </c>
-      <c r="B201" t="inlineStr"/>
-      <c r="C201" t="inlineStr"/>
-      <c r="D201" t="inlineStr"/>
-      <c r="E201" t="inlineStr"/>
-      <c r="F201" t="inlineStr"/>
-      <c r="G201" t="inlineStr"/>
-      <c r="H201" t="inlineStr"/>
-      <c r="I201" t="inlineStr"/>
-      <c r="J201" t="inlineStr"/>
-      <c r="K201" t="inlineStr"/>
-      <c r="L201" t="inlineStr"/>
-      <c r="M201" t="inlineStr"/>
-      <c r="N201" t="inlineStr"/>
-      <c r="O201" t="inlineStr"/>
-      <c r="P201" t="inlineStr"/>
-      <c r="Q201" t="inlineStr"/>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>hypericum hirsutum</t>
-        </is>
-      </c>
-      <c r="B202" t="inlineStr"/>
-      <c r="C202" t="inlineStr"/>
-      <c r="D202" t="inlineStr"/>
-      <c r="E202" t="inlineStr"/>
-      <c r="F202" t="inlineStr"/>
-      <c r="G202" t="inlineStr"/>
-      <c r="H202" t="inlineStr"/>
-      <c r="I202" t="inlineStr"/>
-      <c r="J202" t="inlineStr"/>
-      <c r="K202" t="inlineStr"/>
-      <c r="L202" t="inlineStr"/>
-      <c r="M202" t="inlineStr"/>
-      <c r="N202" t="inlineStr"/>
-      <c r="O202" t="inlineStr"/>
-      <c r="P202" t="inlineStr"/>
-      <c r="Q202" t="inlineStr"/>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>hypochaeris glabra</t>
-        </is>
-      </c>
-      <c r="B203" t="inlineStr"/>
-      <c r="C203" t="inlineStr"/>
-      <c r="D203" t="inlineStr"/>
-      <c r="E203" t="inlineStr"/>
-      <c r="F203" t="inlineStr"/>
-      <c r="G203" t="inlineStr"/>
-      <c r="H203" t="inlineStr"/>
-      <c r="I203" t="inlineStr"/>
-      <c r="J203" t="inlineStr"/>
-      <c r="K203" t="inlineStr"/>
-      <c r="L203" t="inlineStr"/>
-      <c r="M203" t="inlineStr"/>
-      <c r="N203" t="inlineStr"/>
-      <c r="O203" t="inlineStr"/>
-      <c r="P203" t="inlineStr"/>
-      <c r="Q203" t="inlineStr"/>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>leucanthemum vulgare</t>
-        </is>
-      </c>
-      <c r="B204" t="inlineStr"/>
-      <c r="C204" t="inlineStr"/>
-      <c r="D204" t="inlineStr"/>
-      <c r="E204" t="inlineStr"/>
-      <c r="F204" t="inlineStr"/>
-      <c r="G204" t="n">
-        <v>1</v>
-      </c>
-      <c r="H204" t="n">
-        <v>1</v>
-      </c>
-      <c r="I204" t="inlineStr"/>
-      <c r="J204" t="inlineStr"/>
-      <c r="K204" t="inlineStr"/>
-      <c r="L204" t="inlineStr"/>
-      <c r="M204" t="inlineStr"/>
-      <c r="N204" t="inlineStr"/>
-      <c r="O204" t="inlineStr"/>
-      <c r="P204" t="inlineStr"/>
-      <c r="Q204" t="inlineStr"/>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>linaria vulgaris</t>
-        </is>
-      </c>
-      <c r="B205" t="inlineStr"/>
-      <c r="C205" t="inlineStr"/>
-      <c r="D205" t="inlineStr"/>
-      <c r="E205" t="inlineStr"/>
-      <c r="F205" t="inlineStr"/>
-      <c r="G205" t="inlineStr"/>
-      <c r="H205" t="inlineStr"/>
-      <c r="I205" t="inlineStr"/>
-      <c r="J205" t="inlineStr"/>
-      <c r="K205" t="inlineStr"/>
-      <c r="L205" t="inlineStr"/>
-      <c r="M205" t="inlineStr"/>
-      <c r="N205" t="inlineStr"/>
-      <c r="O205" t="inlineStr"/>
-      <c r="P205" t="inlineStr"/>
-      <c r="Q205" t="inlineStr"/>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>phleum</t>
-        </is>
-      </c>
-      <c r="B206" t="inlineStr"/>
-      <c r="C206" t="inlineStr"/>
-      <c r="D206" t="inlineStr"/>
-      <c r="E206" t="inlineStr"/>
-      <c r="F206" t="inlineStr"/>
-      <c r="G206" t="inlineStr"/>
-      <c r="H206" t="inlineStr"/>
-      <c r="I206" t="inlineStr"/>
-      <c r="J206" t="inlineStr"/>
-      <c r="K206" t="inlineStr"/>
-      <c r="L206" t="inlineStr"/>
-      <c r="M206" t="inlineStr"/>
-      <c r="N206" t="inlineStr"/>
-      <c r="O206" t="inlineStr"/>
-      <c r="P206" t="inlineStr"/>
-      <c r="Q206" t="inlineStr"/>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>pilosella officinarum (hieracium)</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr"/>
-      <c r="C207" t="inlineStr"/>
-      <c r="D207" t="inlineStr"/>
-      <c r="E207" t="inlineStr"/>
-      <c r="F207" t="inlineStr"/>
-      <c r="G207" t="n">
-        <v>1</v>
-      </c>
-      <c r="H207" t="n">
-        <v>1</v>
-      </c>
-      <c r="I207" t="inlineStr"/>
-      <c r="J207" t="inlineStr"/>
-      <c r="K207" t="inlineStr"/>
-      <c r="L207" t="inlineStr"/>
-      <c r="M207" t="inlineStr"/>
-      <c r="N207" t="inlineStr"/>
-      <c r="O207" t="inlineStr"/>
-      <c r="P207" t="inlineStr"/>
-      <c r="Q207" t="inlineStr"/>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>plagiomnium affine</t>
-        </is>
-      </c>
-      <c r="B208" t="inlineStr"/>
-      <c r="C208" t="inlineStr"/>
-      <c r="D208" t="inlineStr"/>
-      <c r="E208" t="inlineStr"/>
-      <c r="F208" t="inlineStr"/>
-      <c r="G208" t="inlineStr"/>
-      <c r="H208" t="inlineStr"/>
-      <c r="I208" t="inlineStr"/>
-      <c r="J208" t="inlineStr"/>
-      <c r="K208" t="inlineStr"/>
-      <c r="L208" t="inlineStr"/>
-      <c r="M208" t="inlineStr"/>
-      <c r="N208" t="inlineStr"/>
-      <c r="O208" t="inlineStr"/>
-      <c r="P208" t="inlineStr"/>
-      <c r="Q208" t="inlineStr"/>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>plagiomnium undulatum</t>
-        </is>
-      </c>
-      <c r="B209" t="inlineStr"/>
-      <c r="C209" t="inlineStr"/>
-      <c r="D209" t="inlineStr"/>
-      <c r="E209" t="inlineStr"/>
-      <c r="F209" t="inlineStr"/>
-      <c r="G209" t="inlineStr"/>
-      <c r="H209" t="inlineStr"/>
-      <c r="I209" t="inlineStr"/>
-      <c r="J209" t="inlineStr"/>
-      <c r="K209" t="inlineStr"/>
-      <c r="L209" t="inlineStr"/>
-      <c r="M209" t="inlineStr"/>
-      <c r="N209" t="inlineStr"/>
-      <c r="O209" t="inlineStr"/>
-      <c r="P209" t="inlineStr"/>
-      <c r="Q209" t="inlineStr"/>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>poterium sanguisorba</t>
-        </is>
-      </c>
-      <c r="B210" t="inlineStr"/>
-      <c r="C210" t="inlineStr"/>
-      <c r="D210" t="inlineStr"/>
-      <c r="E210" t="inlineStr"/>
-      <c r="F210" t="inlineStr"/>
-      <c r="G210" t="inlineStr"/>
-      <c r="H210" t="inlineStr"/>
-      <c r="I210" t="inlineStr"/>
-      <c r="J210" t="inlineStr"/>
-      <c r="K210" t="inlineStr"/>
-      <c r="L210" t="inlineStr"/>
-      <c r="M210" t="inlineStr"/>
-      <c r="N210" t="inlineStr"/>
-      <c r="O210" t="inlineStr"/>
-      <c r="P210" t="inlineStr"/>
-      <c r="Q210" t="inlineStr"/>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>prunus domestica</t>
-        </is>
-      </c>
-      <c r="B211" t="inlineStr"/>
-      <c r="C211" t="inlineStr"/>
-      <c r="D211" t="inlineStr"/>
-      <c r="E211" t="inlineStr"/>
-      <c r="F211" t="inlineStr"/>
-      <c r="G211" t="inlineStr"/>
-      <c r="H211" t="inlineStr"/>
-      <c r="I211" t="inlineStr"/>
-      <c r="J211" t="inlineStr"/>
-      <c r="K211" t="inlineStr"/>
-      <c r="L211" t="inlineStr"/>
-      <c r="M211" t="inlineStr"/>
-      <c r="N211" t="inlineStr"/>
-      <c r="O211" t="inlineStr"/>
-      <c r="P211" t="inlineStr"/>
-      <c r="Q211" t="inlineStr"/>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>quercus robur (g)</t>
-        </is>
-      </c>
-      <c r="B212" t="inlineStr"/>
-      <c r="C212" t="inlineStr"/>
-      <c r="D212" t="inlineStr"/>
-      <c r="E212" t="inlineStr"/>
-      <c r="F212" t="inlineStr"/>
-      <c r="G212" t="inlineStr"/>
-      <c r="H212" t="inlineStr"/>
-      <c r="I212" t="inlineStr"/>
-      <c r="J212" t="inlineStr"/>
-      <c r="K212" t="inlineStr"/>
-      <c r="L212" t="inlineStr"/>
-      <c r="M212" t="inlineStr"/>
-      <c r="N212" t="inlineStr"/>
-      <c r="O212" t="inlineStr"/>
-      <c r="P212" t="inlineStr"/>
-      <c r="Q212" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>rubus fruticosus agg. (g)</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr"/>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="inlineStr"/>
-      <c r="E213" t="inlineStr"/>
-      <c r="F213" t="inlineStr"/>
-      <c r="G213" t="inlineStr"/>
-      <c r="H213" t="inlineStr"/>
-      <c r="I213" t="inlineStr"/>
-      <c r="J213" t="inlineStr"/>
-      <c r="K213" t="inlineStr"/>
-      <c r="L213" t="inlineStr"/>
-      <c r="M213" t="inlineStr"/>
-      <c r="N213" t="inlineStr"/>
-      <c r="O213" t="inlineStr"/>
-      <c r="P213" t="inlineStr"/>
-      <c r="Q213" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>scabiosa columbaria</t>
-        </is>
-      </c>
-      <c r="B214" t="inlineStr"/>
-      <c r="C214" t="inlineStr"/>
-      <c r="D214" t="inlineStr"/>
-      <c r="E214" t="inlineStr"/>
-      <c r="F214" t="inlineStr"/>
-      <c r="G214" t="n">
-        <v>1</v>
-      </c>
-      <c r="H214" t="n">
-        <v>1</v>
-      </c>
-      <c r="I214" t="inlineStr"/>
-      <c r="J214" t="inlineStr"/>
-      <c r="K214" t="inlineStr"/>
-      <c r="L214" t="inlineStr"/>
-      <c r="M214" t="inlineStr"/>
-      <c r="N214" t="inlineStr"/>
-      <c r="O214" t="inlineStr"/>
-      <c r="P214" t="inlineStr"/>
-      <c r="Q214" t="inlineStr"/>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>scorzoneroides autumnalis</t>
-        </is>
-      </c>
-      <c r="B215" t="inlineStr"/>
-      <c r="C215" t="inlineStr"/>
-      <c r="D215" t="inlineStr"/>
-      <c r="E215" t="inlineStr"/>
-      <c r="F215" t="inlineStr"/>
-      <c r="G215" t="inlineStr"/>
-      <c r="H215" t="inlineStr"/>
-      <c r="I215" t="inlineStr"/>
-      <c r="J215" t="inlineStr"/>
-      <c r="K215" t="inlineStr"/>
-      <c r="L215" t="inlineStr"/>
-      <c r="M215" t="inlineStr"/>
-      <c r="N215" t="inlineStr"/>
-      <c r="O215" t="inlineStr"/>
-      <c r="P215" t="inlineStr"/>
-      <c r="Q215" t="inlineStr"/>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>silene dioica</t>
-        </is>
-      </c>
-      <c r="B216" t="inlineStr"/>
-      <c r="C216" t="inlineStr"/>
-      <c r="D216" t="inlineStr"/>
-      <c r="E216" t="inlineStr"/>
-      <c r="F216" t="inlineStr"/>
-      <c r="G216" t="inlineStr"/>
-      <c r="H216" t="inlineStr"/>
-      <c r="I216" t="inlineStr"/>
-      <c r="J216" t="inlineStr"/>
-      <c r="K216" t="inlineStr"/>
-      <c r="L216" t="inlineStr"/>
-      <c r="M216" t="inlineStr"/>
-      <c r="N216" t="inlineStr"/>
-      <c r="O216" t="inlineStr"/>
-      <c r="P216" t="inlineStr"/>
-      <c r="Q216" t="inlineStr"/>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>taraxacum</t>
-        </is>
-      </c>
-      <c r="B217" t="inlineStr"/>
-      <c r="C217" t="inlineStr"/>
-      <c r="D217" t="inlineStr"/>
-      <c r="E217" t="inlineStr"/>
-      <c r="F217" t="inlineStr"/>
-      <c r="G217" t="inlineStr"/>
-      <c r="H217" t="inlineStr"/>
-      <c r="I217" t="inlineStr"/>
-      <c r="J217" t="inlineStr"/>
-      <c r="K217" t="inlineStr"/>
-      <c r="L217" t="inlineStr"/>
-      <c r="M217" t="inlineStr"/>
-      <c r="N217" t="inlineStr"/>
-      <c r="O217" t="inlineStr"/>
-      <c r="P217" t="inlineStr"/>
-      <c r="Q217" t="inlineStr"/>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>tragopogon pratensis</t>
-        </is>
-      </c>
-      <c r="B218" t="inlineStr"/>
-      <c r="C218" t="inlineStr"/>
-      <c r="D218" t="inlineStr"/>
-      <c r="E218" t="inlineStr"/>
-      <c r="F218" t="inlineStr"/>
-      <c r="G218" t="inlineStr"/>
-      <c r="H218" t="inlineStr"/>
-      <c r="I218" t="inlineStr"/>
-      <c r="J218" t="inlineStr"/>
-      <c r="K218" t="inlineStr"/>
-      <c r="L218" t="inlineStr"/>
-      <c r="M218" t="inlineStr"/>
-      <c r="N218" t="inlineStr"/>
-      <c r="O218" t="inlineStr"/>
-      <c r="P218" t="inlineStr"/>
-      <c r="Q218" t="inlineStr"/>
-    </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>trifolium hybridum</t>
-        </is>
-      </c>
-      <c r="B219" t="inlineStr"/>
-      <c r="C219" t="inlineStr"/>
-      <c r="D219" t="inlineStr"/>
-      <c r="E219" t="inlineStr"/>
-      <c r="F219" t="inlineStr"/>
-      <c r="G219" t="inlineStr"/>
-      <c r="H219" t="inlineStr"/>
-      <c r="I219" t="inlineStr"/>
-      <c r="J219" t="inlineStr"/>
-      <c r="K219" t="inlineStr"/>
-      <c r="L219" t="inlineStr"/>
-      <c r="M219" t="inlineStr"/>
-      <c r="N219" t="inlineStr"/>
-      <c r="O219" t="inlineStr"/>
-      <c r="P219" t="inlineStr"/>
-      <c r="Q219" t="inlineStr"/>
-    </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>trifolium seedling</t>
-        </is>
-      </c>
-      <c r="B220" t="inlineStr"/>
-      <c r="C220" t="inlineStr"/>
-      <c r="D220" t="inlineStr"/>
-      <c r="E220" t="inlineStr"/>
-      <c r="F220" t="inlineStr"/>
-      <c r="G220" t="inlineStr"/>
-      <c r="H220" t="inlineStr"/>
-      <c r="I220" t="inlineStr"/>
-      <c r="J220" t="inlineStr"/>
-      <c r="K220" t="inlineStr"/>
-      <c r="L220" t="inlineStr"/>
-      <c r="M220" t="inlineStr"/>
-      <c r="N220" t="inlineStr"/>
-      <c r="O220" t="inlineStr"/>
-      <c r="P220" t="inlineStr"/>
-      <c r="Q220" t="inlineStr"/>
-    </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>trisetum flavescens</t>
-        </is>
-      </c>
-      <c r="B221" t="inlineStr"/>
-      <c r="C221" t="inlineStr"/>
-      <c r="D221" t="inlineStr"/>
-      <c r="E221" t="inlineStr"/>
-      <c r="F221" t="inlineStr"/>
-      <c r="G221" t="inlineStr"/>
-      <c r="H221" t="inlineStr"/>
-      <c r="I221" t="inlineStr"/>
-      <c r="J221" t="inlineStr"/>
-      <c r="K221" t="inlineStr"/>
-      <c r="L221" t="inlineStr"/>
-      <c r="M221" t="inlineStr"/>
-      <c r="N221" t="inlineStr"/>
-      <c r="O221" t="inlineStr"/>
-      <c r="P221" t="inlineStr"/>
-      <c r="Q221" t="inlineStr"/>
-    </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>veronica montana</t>
-        </is>
-      </c>
-      <c r="B222" t="inlineStr"/>
-      <c r="C222" t="inlineStr"/>
-      <c r="D222" t="inlineStr"/>
-      <c r="E222" t="inlineStr"/>
-      <c r="F222" t="inlineStr"/>
-      <c r="G222" t="inlineStr"/>
-      <c r="H222" t="inlineStr"/>
-      <c r="I222" t="inlineStr"/>
-      <c r="J222" t="inlineStr"/>
-      <c r="K222" t="inlineStr"/>
-      <c r="L222" t="inlineStr"/>
-      <c r="M222" t="inlineStr"/>
-      <c r="N222" t="inlineStr"/>
-      <c r="O222" t="inlineStr"/>
-      <c r="P222" t="inlineStr"/>
-      <c r="Q222" t="inlineStr"/>
-    </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>vicia sativa</t>
-        </is>
-      </c>
-      <c r="B223" t="inlineStr"/>
-      <c r="C223" t="inlineStr"/>
-      <c r="D223" t="inlineStr"/>
-      <c r="E223" t="inlineStr"/>
-      <c r="F223" t="inlineStr"/>
-      <c r="G223" t="inlineStr"/>
-      <c r="H223" t="inlineStr"/>
-      <c r="I223" t="inlineStr"/>
-      <c r="J223" t="inlineStr"/>
-      <c r="K223" t="inlineStr"/>
-      <c r="L223" t="inlineStr"/>
-      <c r="M223" t="inlineStr"/>
-      <c r="N223" t="inlineStr"/>
-      <c r="O223" t="inlineStr"/>
-      <c r="P223" t="inlineStr"/>
-      <c r="Q223" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>